<commit_message>
19.03.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/March/All Details/19.03.2020/MC Balance Transfer March 2020.xlsx
+++ b/2020/March/All Details/19.03.2020/MC Balance Transfer March 2020.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="101">
   <si>
     <t>Date</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>Shohel Store</t>
+  </si>
+  <si>
+    <t>19.03.2020</t>
+  </si>
+  <si>
+    <t>Galaxy</t>
+  </si>
+  <si>
+    <t>Dsr Murad</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1112,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1115,7 +1124,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1138,14 +1147,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1453,9 +1462,9 @@
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomLeft" activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -3016,21 +3025,33 @@
       <c r="BI20" s="7"/>
     </row>
     <row r="21" spans="1:61" ht="12.6" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="A21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="2">
+        <v>258280</v>
+      </c>
+      <c r="C21" s="2">
+        <v>256255</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2100</v>
+      </c>
       <c r="E21" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>258355</v>
       </c>
       <c r="F21" s="99"/>
       <c r="G21" s="17"/>
       <c r="H21" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
+      <c r="I21" s="51">
+        <v>1050</v>
+      </c>
+      <c r="J21" s="51" t="s">
+        <v>98</v>
+      </c>
       <c r="K21" s="96"/>
       <c r="L21" s="40"/>
       <c r="M21" s="7"/>
@@ -3835,23 +3856,23 @@
       </c>
       <c r="B33" s="2">
         <f>SUM(B5:B32)</f>
-        <v>5521710</v>
+        <v>5779990</v>
       </c>
       <c r="C33" s="2">
         <f>SUM(C5:C32)</f>
-        <v>5582446</v>
+        <v>5838701</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D5:D32)</f>
-        <v>17577</v>
+        <v>19677</v>
       </c>
       <c r="E33" s="2">
         <f>SUM(E5:E32)</f>
-        <v>5600023</v>
+        <v>5858378</v>
       </c>
       <c r="F33" s="69">
         <f>B33-E33</f>
-        <v>-78313</v>
+        <v>-78388</v>
       </c>
       <c r="G33" s="85"/>
       <c r="H33" s="90" t="s">
@@ -4353,10 +4374,10 @@
         <v>36</v>
       </c>
       <c r="C40" s="2">
-        <v>15420</v>
+        <v>15720</v>
       </c>
       <c r="D40" s="126" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="99"/>
@@ -4634,7 +4655,7 @@
       <c r="A44" s="120"/>
       <c r="B44" s="121"/>
       <c r="C44" s="122">
-        <v>2763</v>
+        <v>883</v>
       </c>
       <c r="D44" s="123"/>
       <c r="E44" s="3"/>
@@ -4830,10 +4851,10 @@
       </c>
       <c r="B47" s="72"/>
       <c r="C47" s="73">
-        <v>114000</v>
+        <v>100000</v>
       </c>
       <c r="D47" s="74" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="113"/>
@@ -5102,10 +5123,10 @@
       </c>
       <c r="B51" s="32"/>
       <c r="C51" s="73">
-        <v>415255</v>
+        <v>381135</v>
       </c>
       <c r="D51" s="74" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="32"/>
@@ -5171,10 +5192,10 @@
       </c>
       <c r="B52" s="32"/>
       <c r="C52" s="73">
-        <v>196050</v>
+        <v>196350</v>
       </c>
       <c r="D52" s="133" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="113"/>
@@ -5725,10 +5746,10 @@
       </c>
       <c r="B60" s="32"/>
       <c r="C60" s="73">
-        <v>232000</v>
+        <v>267000</v>
       </c>
       <c r="D60" s="74" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="32"/>
@@ -5860,10 +5881,16 @@
       <c r="BI61" s="7"/>
     </row>
     <row r="62" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A62" s="75"/>
+      <c r="A62" s="75" t="s">
+        <v>99</v>
+      </c>
       <c r="B62" s="32"/>
-      <c r="C62" s="73"/>
-      <c r="D62" s="74"/>
+      <c r="C62" s="73">
+        <v>13325</v>
+      </c>
+      <c r="D62" s="74" t="s">
+        <v>98</v>
+      </c>
       <c r="E62" s="8"/>
       <c r="F62" s="143" t="s">
         <v>24</v>
@@ -5931,10 +5958,16 @@
       <c r="BI62" s="7"/>
     </row>
     <row r="63" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A63" s="75"/>
+      <c r="A63" s="75" t="s">
+        <v>100</v>
+      </c>
       <c r="B63" s="32"/>
-      <c r="C63" s="73"/>
-      <c r="D63" s="74"/>
+      <c r="C63" s="73">
+        <v>1000</v>
+      </c>
+      <c r="D63" s="74" t="s">
+        <v>98</v>
+      </c>
       <c r="E63" s="3"/>
       <c r="F63" s="50"/>
       <c r="G63" s="13"/>
@@ -8539,7 +8572,7 @@
       <c r="B98" s="142"/>
       <c r="C98" s="34">
         <f>SUM(C37:C97)</f>
-        <v>1959132</v>
+        <v>1959057</v>
       </c>
       <c r="D98" s="30"/>
       <c r="F98" s="114"/>
@@ -8674,7 +8707,7 @@
       <c r="B100" s="140"/>
       <c r="C100" s="31">
         <f>C98+L121</f>
-        <v>1959132</v>
+        <v>1959057</v>
       </c>
       <c r="D100" s="21"/>
       <c r="F100" s="50"/>

</xml_diff>